<commit_message>
User details recorder search implemented
</commit_message>
<xml_diff>
--- a/User.xlsx
+++ b/User.xlsx
@@ -38,31 +38,28 @@
     <t xml:space="preserve">MOB</t>
   </si>
   <si>
-    <t xml:space="preserve">gf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hgfh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gfnnn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hfhg</t>
+    <t xml:space="preserve">SJ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das@dfg.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">413548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ3</t>
   </si>
   <si>
     <t xml:space="preserve">alok</t>
   </si>
   <si>
-    <t xml:space="preserve">dd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ss</t>
+    <t xml:space="preserve">alohg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65674537</t>
   </si>
 </sst>
 </file>
@@ -402,59 +399,31 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="D2">
+        <v>413548</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>3</v>
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day book added icons updated
</commit_message>
<xml_diff>
--- a/User.xlsx
+++ b/User.xlsx
@@ -60,6 +60,42 @@
   </si>
   <si>
     <t xml:space="preserve">65674537</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vijay 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jhgyg@jjhj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1214512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r16@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">879545756454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SJ6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thullu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsfd@dfs.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45468645454</t>
   </si>
 </sst>
 </file>
@@ -422,8 +458,50 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="D3">
+        <v>65674537</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>1214512</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>879545756454</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>